<commit_message>
Added cell classes and groups
</commit_message>
<xml_diff>
--- a/Data/xlsx/basal_ganglia_regions.xlsx
+++ b/Data/xlsx/basal_ganglia_regions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\solutions\uio\master\jup_bg\Data\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF4E56A-769E-45D7-A883-5DC19901CB48}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35E6639D-B368-4271-AE3F-2F9845D21FBE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23136" yWindow="-1974" windowWidth="23232" windowHeight="12552" activeTab="6" xr2:uid="{113542D8-D7D4-4518-AD00-840EFC990A81}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{113542D8-D7D4-4518-AD00-840EFC990A81}"/>
   </bookViews>
   <sheets>
     <sheet name="regions_other" sheetId="1" r:id="rId1"/>
@@ -35964,13 +35964,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DADF396D-6192-40B2-8516-0125D856C777}">
-  <dimension ref="A1:C31"/>
+  <dimension ref="A1:C33"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L27" sqref="L27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="28.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -36287,8 +36290,8 @@
       <c r="B29" t="s">
         <v>1025</v>
       </c>
-      <c r="C29" t="s">
-        <v>31</v>
+      <c r="C29">
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -36298,8 +36301,8 @@
       <c r="B30" t="s">
         <v>1026</v>
       </c>
-      <c r="C30" t="s">
-        <v>31</v>
+      <c r="C30">
+        <v>2</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
@@ -36311,6 +36314,28 @@
       </c>
       <c r="C31">
         <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>36</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1025</v>
+      </c>
+      <c r="C32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>37</v>
+      </c>
+      <c r="B33" t="s">
+        <v>1026</v>
+      </c>
+      <c r="C33">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
@@ -37348,8 +37373,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49CEB101-7584-4CC7-9BE2-EC44B9608990}">
   <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:H17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>